<commit_message>
Updates for Rev 2 of manuscript
new images and new edits
also added comments for referees
</commit_message>
<xml_diff>
--- a/BMA_Hydration/data/Model_Metadata.xlsx
+++ b/BMA_Hydration/data/Model_Metadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26621"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="42240" yWindow="0" windowWidth="25780" windowHeight="16720"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Model_Metadata" sheetId="1" r:id="rId1"/>
@@ -224,9 +224,6 @@
     <t>alc-1</t>
   </si>
   <si>
-    <t>exp-2</t>
-  </si>
-  <si>
     <t>alc-2</t>
   </si>
   <si>
@@ -261,6 +258,9 @@
   </si>
   <si>
     <t>exp-4</t>
+  </si>
+  <si>
+    <t>hyb-2</t>
   </si>
 </sst>
 </file>
@@ -623,7 +623,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -763,7 +763,7 @@
         <v>2</v>
       </c>
       <c r="H5" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -789,7 +789,7 @@
         <v>3</v>
       </c>
       <c r="H6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -815,7 +815,7 @@
         <v>3</v>
       </c>
       <c r="H7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -841,7 +841,7 @@
         <v>3</v>
       </c>
       <c r="H8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -867,7 +867,7 @@
         <v>3</v>
       </c>
       <c r="H9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -893,7 +893,7 @@
         <v>1</v>
       </c>
       <c r="H10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -919,7 +919,7 @@
         <v>1</v>
       </c>
       <c r="H11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -945,7 +945,7 @@
         <v>1</v>
       </c>
       <c r="H12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -971,7 +971,7 @@
         <v>1</v>
       </c>
       <c r="H13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -997,7 +997,7 @@
         <v>1</v>
       </c>
       <c r="H14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1023,7 +1023,7 @@
         <v>2</v>
       </c>
       <c r="H15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1049,7 +1049,7 @@
         <v>1</v>
       </c>
       <c r="H16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1075,7 +1075,7 @@
         <v>1</v>
       </c>
       <c r="H17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -1089,7 +1089,7 @@
         <v>2</v>
       </c>
       <c r="H18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>